<commit_message>
measure input pulse ok
</commit_message>
<xml_diff>
--- a/Estimate_DTG1.xlsx
+++ b/Estimate_DTG1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\BYT-Hawaco-GW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD91844F-FAA9-4AE2-B90C-072A9AC33007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBEF26CC-007D-40CC-B414-5A3752471062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E3B0EE95-4F77-45F0-A084-54B3AA7279E9}"/>
   </bookViews>
@@ -611,7 +611,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +658,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="3">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -679,7 +679,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="3">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="3">
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -709,7 +709,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="9">
-        <v>96</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
       </c>
       <c r="D11" s="7">
         <f>(86400000-D2*D4-D7*D5-D21*D22)</f>
-        <v>85625200</v>
+        <v>85737200</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
         <v>32</v>
       </c>
       <c r="D13" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -830,7 +830,7 @@
       </c>
       <c r="D19" s="5">
         <f>(D3*D2*D4+D5*D7*D6+D11*D12)/86400000</f>
-        <v>22.825277777777778</v>
+        <v>20.133611111111112</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -844,7 +844,7 @@
         <v>21</v>
       </c>
       <c r="D20" s="3">
-        <v>50000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -854,7 +854,7 @@
         <v>16</v>
       </c>
       <c r="D21" s="3">
-        <v>30000</v>
+        <v>27000</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -877,7 +877,7 @@
       </c>
       <c r="D23" s="5">
         <f>D20*D21*D22/86400000</f>
-        <v>416.66666666666669</v>
+        <v>750</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -892,7 +892,7 @@
       </c>
       <c r="D24" s="5">
         <f>24*(D23+D19)/1000 + D10*D9/3600/1000 +D13*D14*D15/3600/1000 + D16*D17*D18/3600/1000</f>
-        <v>10.787920555555557</v>
+        <v>18.723287222222218</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -939,7 +939,7 @@
       </c>
       <c r="D28" s="8">
         <f>D26*D27*D25/4.2/(D24*30)</f>
-        <v>35.018591009481433</v>
+        <v>20.176893795091836</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>